<commit_message>
Changes to plots and adding block analysis
</commit_message>
<xml_diff>
--- a/writing/Table1_ANOVA.xlsx
+++ b/writing/Table1_ANOVA.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moin2\OneDrive\Documents\Horsenettle\writing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB98B4D2-6F07-40DF-9FB5-BBBA9DF51614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F13E5D-9405-452C-A472-7B2BFE2FB17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="312" yWindow="3132" windowWidth="17280" windowHeight="8964" xr2:uid="{32E11D0F-C2D5-496D-A17A-BB60A8075FD3}"/>
+    <workbookView xWindow="-5352" yWindow="3408" windowWidth="17280" windowHeight="8964" xr2:uid="{32E11D0F-C2D5-496D-A17A-BB60A8075FD3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="LM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="33">
   <si>
     <t>Variable</t>
   </si>
@@ -94,29 +95,56 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>More Tolerant</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>South</t>
-  </si>
-  <si>
-    <t>North</t>
-  </si>
-  <si>
     <t>Chlorophyll Fluorescence (Heat)</t>
   </si>
   <si>
     <t>Chlorophyll Fluorescence (Cold)</t>
+  </si>
+  <si>
+    <t>F-value</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Random Effects</t>
+  </si>
+  <si>
+    <t>Population: ID</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>LRT</t>
+  </si>
+  <si>
+    <t>Expectations</t>
+  </si>
+  <si>
+    <t>Observed</t>
+  </si>
+  <si>
+    <t>S &gt; N</t>
+  </si>
+  <si>
+    <t>N &gt; S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +173,26 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -154,74 +202,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -243,37 +229,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <left/>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left/>
+      <right/>
+      <top style="thick">
         <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -283,74 +254,127 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -669,306 +693,308 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F32102E-11BC-48ED-855E-8F81D68DDEB9}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B1" s="11"/>
-      <c r="C1" s="26" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="45"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="26" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="28"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="3">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="C3" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="29">
+        <v>6.1019999999999998E-2</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="20">
-        <v>2.1000000000000001E-2</v>
+      <c r="G3" s="42">
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="20">
-        <v>6.0000000000000001E-3</v>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="40">
+        <v>1.17E-2</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="3">
-        <v>0.86</v>
+      <c r="G4" s="17">
+        <v>0.88600000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="20">
-        <v>4.2999999999999997E-2</v>
+      <c r="A5" s="34"/>
+      <c r="B5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="40">
+        <v>0.40500000000000003</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="3">
-        <v>0.36399999999999999</v>
+      <c r="G5" s="17">
+        <v>0.38</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
-      <c r="B6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="41">
+        <v>9.9599999999999997E-11</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="21">
-        <v>4.1790000000000003E-10</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="21">
-        <v>6.1399999999999999E-9</v>
+      <c r="G6" s="41">
+        <v>1.05E-7</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="34"/>
+      <c r="B7" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.76800000000000002</v>
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0.997</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="3">
-        <v>0.64300000000000002</v>
+      <c r="G7" s="17">
+        <v>0.127</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="35"/>
+      <c r="B8" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="27">
+        <v>0.77</v>
+      </c>
+      <c r="F8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.442</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.89200000000000002</v>
+      <c r="G8" s="27">
+        <v>0.88300000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="34" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="40">
+        <v>3.6999999999999999E-4</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="22">
-        <v>3.6999999999999999E-4</v>
-      </c>
-      <c r="F9" s="15" t="s">
+      <c r="G9" s="40">
+        <v>2.5100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="34"/>
+      <c r="B10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="40">
+        <v>6.8499999999999995E-4</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="22">
-        <v>2.5100000000000001E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="18" t="s">
+      <c r="G10" s="40">
+        <v>3.5099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="34"/>
+      <c r="B11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="20">
-        <v>6.8499999999999995E-4</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="20">
-        <v>3.5099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
-      <c r="B11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.33100000000000002</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="21">
+      <c r="G11" s="41">
         <v>8.7100000000000006E-8</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="34"/>
+      <c r="B12" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="3">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="17">
         <v>0.56799999999999995</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="17">
         <v>0.41799999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="34"/>
+      <c r="B13" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="3">
+        <v>31</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="17">
         <v>0.77</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="17">
         <v>0.60799999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="35"/>
+      <c r="B14" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="27">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="F14" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="5">
+      <c r="G14" s="27">
         <v>0.496</v>
       </c>
     </row>
@@ -981,4 +1007,425 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F850DF-B4C3-4116-99E5-F83F0B438EEA}">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="32"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+    </row>
+    <row r="2" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="25"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="36"/>
+    </row>
+    <row r="3" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="25"/>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3.6732999999999998</v>
+      </c>
+      <c r="D4" s="6">
+        <v>49.948</v>
+      </c>
+      <c r="E4" s="6">
+        <v>6.1019999999999998E-2</v>
+      </c>
+      <c r="F4" s="30">
+        <v>4.7282999999999999</v>
+      </c>
+      <c r="G4" s="30">
+        <v>2.9669999999999998E-2</v>
+      </c>
+      <c r="H4" s="6">
+        <v>3.3197999999999999</v>
+      </c>
+      <c r="I4" s="6">
+        <v>6.8449999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="34"/>
+      <c r="B5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14">
+        <v>6.4819000000000004</v>
+      </c>
+      <c r="D5" s="14">
+        <v>191.02</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1.1690000000000001E-2</v>
+      </c>
+      <c r="F5" s="14">
+        <v>15.731</v>
+      </c>
+      <c r="G5" s="19">
+        <v>7.3009999999999994E-5</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="34"/>
+      <c r="B6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="14">
+        <v>4.4180999999999999</v>
+      </c>
+      <c r="D6" s="14">
+        <v>51.122</v>
+      </c>
+      <c r="E6" s="14">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.222465</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0.63719999999999999</v>
+      </c>
+      <c r="H6" s="18">
+        <v>1.8373E-2</v>
+      </c>
+      <c r="I6" s="18">
+        <v>0.89219999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="34"/>
+      <c r="B7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="13">
+        <v>66.369</v>
+      </c>
+      <c r="D7" s="13">
+        <v>49.933</v>
+      </c>
+      <c r="E7" s="19">
+        <v>9.9670000000000003E-11</v>
+      </c>
+      <c r="F7" s="18">
+        <v>1.0175000000000001</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.31309999999999999</v>
+      </c>
+      <c r="H7" s="18">
+        <v>2.0823</v>
+      </c>
+      <c r="I7" s="18">
+        <v>0.14899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="34"/>
+      <c r="B8" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="20">
+        <v>1.2398000000000001E-5</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.997</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="35"/>
+      <c r="B9" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="31">
+        <v>3.2694000000000001</v>
+      </c>
+      <c r="D9" s="8">
+        <v>46.752000000000002</v>
+      </c>
+      <c r="E9" s="8">
+        <v>7.7020000000000005E-2</v>
+      </c>
+      <c r="F9" s="31">
+        <v>0.14763999999999999</v>
+      </c>
+      <c r="G9" s="31">
+        <v>0.70079999999999998</v>
+      </c>
+      <c r="H9" s="31">
+        <v>1.6736</v>
+      </c>
+      <c r="I9" s="31">
+        <v>0.1958</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="22">
+        <v>14.28</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="23">
+        <v>3.6999999999999999E-4</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="34"/>
+      <c r="B11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="22">
+        <v>12.85</v>
+      </c>
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
+      <c r="E11" s="23">
+        <v>6.8499999999999995E-4</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="34"/>
+      <c r="B12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="24">
+        <v>0.96</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
+      <c r="E12" s="24">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="34"/>
+      <c r="B13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="24">
+        <v>0.33</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="34"/>
+      <c r="B14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="24">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="24">
+        <v>0.77</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="35"/>
+      <c r="B15" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="28">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="D15" s="11">
+        <v>1</v>
+      </c>
+      <c r="E15" s="28">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>